<commit_message>
Unirest new version changes
</commit_message>
<xml_diff>
--- a/CasinoGamesAPITest/CasinoGamesAPITest/src/test/java/APICasinoGamesCasinoImagesBrokenData/10bet2winDataBrokenIMGList.xlsx
+++ b/CasinoGamesAPITest/CasinoGamesAPITest/src/test/java/APICasinoGamesCasinoImagesBrokenData/10bet2winDataBrokenIMGList.xlsx
@@ -71,169 +71,169 @@
     <t>221  Game Provider Name = QuickSpin   Game Name =  Durian Dynamite  cod = 404   src = https://resources.bet2win.vip/products/outcomebet/web/DurianDynamite.png</t>
   </si>
   <si>
-    <t>229  Game Provider Name = QuickSpin   Game Name =  Eastern Emeralds  cod = 404   src = https://resources.bet2win.vip/products/outcomebet/web/EasternEmeralds.png</t>
-  </si>
-  <si>
-    <t>246  Game Provider Name = QuickSpin   Game Name =  Fairy Gate  cod = 404   src = https://resources.bet2win.vip/products/outcomebet/web/FairyGate.png</t>
-  </si>
-  <si>
-    <t>259  Game Provider Name = TomHorn   Game Name =  Feng Fu  cod = 404   src = https://resources.bet2win.vip/products/tomhorn/web/FengFu.png</t>
-  </si>
-  <si>
-    <t>266  Game Provider Name = TomHorn   Game Name =  Fire 'n' Hot  cod = 404   src = https://resources.bet2win.vip/products/tomhorn/web/FirenHot.png</t>
-  </si>
-  <si>
-    <t>278  Game Provider Name = TomHorn   Game Name =  Flaming Fruit  cod = 404   src = https://resources.bet2win.vip/products/tomhorn/web/FlamingFruit.png</t>
-  </si>
-  <si>
-    <t>292  Game Provider Name = TomHorn   Game Name =  Frozen Queen  cod = 404   src = https://resources.bet2win.vip/products/tomhorn/web/FrozenQueen.png</t>
-  </si>
-  <si>
-    <t>312  Game Provider Name = TomHorn   Game Name =  Geisha's Fan  cod = 404   src = https://resources.bet2win.vip/products/tomhorn/web/GeishasFun.png</t>
-  </si>
-  <si>
-    <t>318  Game Provider Name = QuickSpin   Game Name =  Genies Touch  cod = 404   src = https://resources.bet2win.vip/products/outcomebet/web/qso_geniestouch.jpg</t>
-  </si>
-  <si>
-    <t>333  Game Provider Name = TomHorn   Game Name =  Gold x  cod = 404   src = https://resources.bet2win.vip/products/tomhorn/web/gold-x.png</t>
-  </si>
-  <si>
-    <t>346  Game Provider Name = QuickSpin   Game Name =  Goldilocks &amp; Wild Bears  cod = 404   src = https://resources.bet2win.vip/products/outcomebet/web/qso_goldilocks2.jpg</t>
-  </si>
-  <si>
-    <t>347  Game Provider Name = QuickSpin   Game Name =  Gold Lab  cod = 404   src = https://resources.bet2win.vip/products/outcomebet/web/qso_goldlab.jpg</t>
-  </si>
-  <si>
-    <t>377  Game Provider Name = TomHorn   Game Name =  Hot Blizzard  cod = 404   src = https://resources.bet2win.vip/products/tomhorn/web/hot-blizzard.png</t>
-  </si>
-  <si>
-    <t>382  Game Provider Name = QuickSpin   Game Name =  Hot Sync  cod = 404   src = https://resources.bet2win.vip/products/outcomebet/web/HotSync.png</t>
-  </si>
-  <si>
-    <t>386  Game Provider Name = TomHorn   Game Name =  Hot'n'Fruity  cod = 404   src = https://resources.bet2win.vip/products/tomhorn/web/hotnfruity.png</t>
-  </si>
-  <si>
-    <t>403  Game Provider Name = QuickSpin   Game Name =  Illuminous  cod = 404   src = https://resources.bet2win.vip/products/outcomebet/web/qso_illuminous.jpg</t>
-  </si>
-  <si>
-    <t>408  Game Provider Name = TomHorn   Game Name =  Inca's Treasure  cod = 404   src = https://resources.bet2win.vip/products/tomhorn/web/incas-treasure.png</t>
-  </si>
-  <si>
-    <t>414  Game Provider Name = RelaxGaming   Game Name =  Iron Bank  cod = 404   src = https://resources.bet2win.vip/products/outcomebet/ironbank_rg.jpg</t>
-  </si>
-  <si>
-    <t>437  Game Provider Name = TomHorn   Game Name =  Joker Reelz  cod = 404   src = https://resources.bet2win.vip/products/tomhorn/web/joker-reelz.png</t>
-  </si>
-  <si>
-    <t>474  Game Provider Name = QuickSpin   Game Name =  Leprechaun Hills  cod = 404   src = https://resources.bet2win.vip/products/outcomebet/web/qso_leprechaunhills.jpg</t>
-  </si>
-  <si>
-    <t>515  Game Provider Name = QuickSpin   Game Name =  Mayana  cod = 404   src = https://resources.bet2win.vip/products/outcomebet/web/qso_mayana.jpg</t>
-  </si>
-  <si>
-    <t>528  Game Provider Name = QuickSpin   Game Name =  Mighty Arthur  cod = 404   src = https://resources.bet2win.vip/products/outcomebet/web/qso_mightyarthur.jpg</t>
-  </si>
-  <si>
-    <t>534  Game Provider Name = RelaxGaming   Game Name =  Money Train 2  cod = 404   src = https://resources.bet2win.vip/products/outcomebet/moneytrain2_rg.jpg</t>
-  </si>
-  <si>
-    <t>535  Game Provider Name = TomHorn   Game Name =  Monkey 27  cod = 404   src = https://resources.bet2win.vip/products/tomhorn/web/Monkey27.png</t>
-  </si>
-  <si>
-    <t>539  Game Provider Name = TomHorn   Game Name =  Monster Madness  cod = 404   src = https://resources.bet2win.vip/products/tomhorn/web/MonsterMadness.png</t>
-  </si>
-  <si>
-    <t>545  Game Provider Name = QuickSpin   Game Name =  Mountain King  cod = 404   src = https://resources.bet2win.vip/products/outcomebet/web/MountainKing.png</t>
-  </si>
-  <si>
-    <t>561  Game Provider Name = QuickSpin   Game Name =  Northern Sky  cod = 404   src = https://resources.bet2win.vip/products/outcomebet/web/NorthernSky.png</t>
-  </si>
-  <si>
-    <t>572  Game Provider Name = TomHorn   Game Name =  Panda's Run  cod = 404   src = https://resources.bet2win.vip/products/tomhorn/web/PandasRun.png</t>
-  </si>
-  <si>
-    <t>585  Game Provider Name = QuickSpin   Game Name =  Phoenix Sun  cod = 404   src = https://resources.bet2win.vip/products/outcomebet/web/qso_phoenixsun.jpg</t>
-  </si>
-  <si>
-    <t>586  Game Provider Name = QuickSpin   Game Name =  Pied Piper  cod = 404   src = https://resources.bet2win.vip/products/outcomebet/web/PiedPiper.png</t>
-  </si>
-  <si>
-    <t>594  Game Provider Name = QuickSpin   Game Name =  Pirates Charm  cod = 404   src = https://resources.bet2win.vip/products/outcomebet/web/PiratesCharm.png</t>
-  </si>
-  <si>
-    <t>626  Game Provider Name = QuickSpin   Game Name =  Razortooth  cod = 404   src = https://resources.bet2win.vip/products/outcomebet/web/qso_sabretooth.jpg</t>
-  </si>
-  <si>
-    <t>629  Game Provider Name = TomHorn   Game Name =  Red Lights  cod = 404   src = https://resources.bet2win.vip/products/tomhorn/web/RedLights.png</t>
-  </si>
-  <si>
-    <t>680  Game Provider Name = TomHorn   Game Name =  Savannah King  cod = 404   src = https://resources.bet2win.vip/products/tomhorn/web/SavannahKing.png</t>
-  </si>
-  <si>
-    <t>681  Game Provider Name = TomHorn   Game Name =  Scratch Card  cod = 404   src = https://resources.bet2win.vip/products/tomhorn/ScratchCard.png</t>
-  </si>
-  <si>
-    <t>686  Game Provider Name = QuickSpin   Game Name =  Second Strike  cod = 404   src = https://resources.bet2win.vip/products/outcomebet/web/qso_secondstrike.jpg</t>
-  </si>
-  <si>
-    <t>693  Game Provider Name = QuickSpin   Game Name =  Sevens High  cod = 404   src = https://resources.bet2win.vip/products/outcomebet/web/qso_sevens.jpg</t>
-  </si>
-  <si>
-    <t>696  Game Provider Name = TomHorn   Game Name =  Shaolin's Tiger  cod = 404   src = https://resources.bet2win.vip/products/tomhorn/web/ShaolinsTiger.jpg</t>
-  </si>
-  <si>
-    <t>698  Game Provider Name = TomHorn   Game Name =  Sherlock in Bohemia  cod = 404   src = https://resources.bet2win.vip/products/tomhorn/web/Sherlock.png</t>
-  </si>
-  <si>
-    <t>702  Game Provider Name = TomHorn   Game Name =  Sizable Win  cod = 404   src = https://resources.bet2win.vip/products/tomhorn/web/SizableWin.png</t>
-  </si>
-  <si>
-    <t>706  Game Provider Name = TomHorn   Game Name =  Sky Barons  cod = 404   src = https://resources.bet2win.vip/products/tomhorn/web/SkyBarons.png</t>
-  </si>
-  <si>
-    <t>709  Game Provider Name = RelaxGaming   Game Name =  Snake Arena  cod = 404   src = https://resources.bet2win.vip/products/outcomebet/snakearena_rg.jpg</t>
-  </si>
-  <si>
-    <t>722  Game Provider Name = TomHorn   Game Name =  Spinball  cod = 404   src = https://resources.bet2win.vip/products/tomhorn/web/spinball.png</t>
-  </si>
-  <si>
-    <t>723  Game Provider Name = QuickSpin   Game Name =  Spinions Beach Party  cod = 404   src = https://resources.bet2win.vip/products/outcomebet/web/qso_spinions.jpg</t>
-  </si>
-  <si>
-    <t>733  Game Provider Name = QuickSpin   Game Name =  Sticky Bandits  cod = 404   src = https://resources.bet2win.vip/products/outcomebet/web/qso_stickybandits.jpg</t>
-  </si>
-  <si>
-    <t>750  Game Provider Name = TomHorn   Game Name =  Sweet Crush  cod = 404   src = https://resources.bet2win.vip/products/tomhorn/web/sweet-crush.png</t>
-  </si>
-  <si>
-    <t>758  Game Provider Name = QuickSpin   Game Name =  Tales of Doctor Dolittle  cod = 404   src = https://resources.bet2win.vip/products/outcomebet/web/TalesofDoctorDolittle.png</t>
-  </si>
-  <si>
-    <t>763  Game Provider Name = TomHorn   Game Name =  The Cup  cod = 404   src = https://resources.bet2win.vip/products/tomhorn/web/TheCup.png</t>
-  </si>
-  <si>
-    <t>787  Game Provider Name = TomHorn   Game Name =  The Secret of BA  cod = 404   src = https://resources.bet2win.vip/products/tomhorn/web/the-secret-of-ba.png</t>
-  </si>
-  <si>
-    <t>795  Game Provider Name = TomHorn   Game Name =  Thrones Of Persia  cod = 404   src = https://resources.bet2win.vip/products/tomhorn/web/ThronesOfPersia.png</t>
-  </si>
-  <si>
-    <t>840  Game Provider Name = QuickSpin   Game Name =  Volcano Riches  cod = 404   src = https://resources.bet2win.vip/products/outcomebet/web/VolcanoRiches.png</t>
-  </si>
-  <si>
-    <t>851  Game Provider Name = RelaxGaming   Game Name =  Wild Chapo  cod = 404   src = https://resources.bet2win.vip/products/outcomebet/wildchapo_rg.jpg</t>
-  </si>
-  <si>
-    <t>853  Game Provider Name = QuickSpin   Game Name =  Wild Chase  cod = 404   src = https://resources.bet2win.vip/products/outcomebet/web/WildChase.png</t>
-  </si>
-  <si>
-    <t>867  Game Provider Name = TomHorn   Game Name =  Wild Weather  cod = 404   src = https://resources.bet2win.vip/products/tomhorn/web/WildWeather.png</t>
-  </si>
-  <si>
-    <t>875  Game Provider Name = QuickSpin   Game Name =  Wins of Fortune  cod = 404   src = https://resources.bet2win.vip/products/outcomebet/web/WinsofFortune.png</t>
-  </si>
-  <si>
-    <t>879  Game Provider Name = TomHorn   Game Name =  Wolf Sierra  cod = 404   src = https://resources.bet2win.vip/products/tomhorn/web/wolf-sierra.png</t>
+    <t>228  Game Provider Name = QuickSpin   Game Name =  Eastern Emeralds  cod = 404   src = https://resources.bet2win.vip/products/outcomebet/web/EasternEmeralds.png</t>
+  </si>
+  <si>
+    <t>245  Game Provider Name = QuickSpin   Game Name =  Fairy Gate  cod = 404   src = https://resources.bet2win.vip/products/outcomebet/web/FairyGate.png</t>
+  </si>
+  <si>
+    <t>258  Game Provider Name = TomHorn   Game Name =  Feng Fu  cod = 404   src = https://resources.bet2win.vip/products/tomhorn/web/FengFu.png</t>
+  </si>
+  <si>
+    <t>265  Game Provider Name = TomHorn   Game Name =  Fire 'n' Hot  cod = 404   src = https://resources.bet2win.vip/products/tomhorn/web/FirenHot.png</t>
+  </si>
+  <si>
+    <t>277  Game Provider Name = TomHorn   Game Name =  Flaming Fruit  cod = 404   src = https://resources.bet2win.vip/products/tomhorn/web/FlamingFruit.png</t>
+  </si>
+  <si>
+    <t>291  Game Provider Name = TomHorn   Game Name =  Frozen Queen  cod = 404   src = https://resources.bet2win.vip/products/tomhorn/web/FrozenQueen.png</t>
+  </si>
+  <si>
+    <t>311  Game Provider Name = TomHorn   Game Name =  Geisha's Fan  cod = 404   src = https://resources.bet2win.vip/products/tomhorn/web/GeishasFun.png</t>
+  </si>
+  <si>
+    <t>317  Game Provider Name = QuickSpin   Game Name =  Genies Touch  cod = 404   src = https://resources.bet2win.vip/products/outcomebet/web/qso_geniestouch.jpg</t>
+  </si>
+  <si>
+    <t>332  Game Provider Name = TomHorn   Game Name =  Gold x  cod = 404   src = https://resources.bet2win.vip/products/tomhorn/web/gold-x.png</t>
+  </si>
+  <si>
+    <t>345  Game Provider Name = QuickSpin   Game Name =  Goldilocks &amp; Wild Bears  cod = 404   src = https://resources.bet2win.vip/products/outcomebet/web/qso_goldilocks2.jpg</t>
+  </si>
+  <si>
+    <t>346  Game Provider Name = QuickSpin   Game Name =  Gold Lab  cod = 404   src = https://resources.bet2win.vip/products/outcomebet/web/qso_goldlab.jpg</t>
+  </si>
+  <si>
+    <t>376  Game Provider Name = TomHorn   Game Name =  Hot Blizzard  cod = 404   src = https://resources.bet2win.vip/products/tomhorn/web/hot-blizzard.png</t>
+  </si>
+  <si>
+    <t>381  Game Provider Name = QuickSpin   Game Name =  Hot Sync  cod = 404   src = https://resources.bet2win.vip/products/outcomebet/web/HotSync.png</t>
+  </si>
+  <si>
+    <t>385  Game Provider Name = TomHorn   Game Name =  Hot'n'Fruity  cod = 404   src = https://resources.bet2win.vip/products/tomhorn/web/hotnfruity.png</t>
+  </si>
+  <si>
+    <t>402  Game Provider Name = QuickSpin   Game Name =  Illuminous  cod = 404   src = https://resources.bet2win.vip/products/outcomebet/web/qso_illuminous.jpg</t>
+  </si>
+  <si>
+    <t>407  Game Provider Name = TomHorn   Game Name =  Inca's Treasure  cod = 404   src = https://resources.bet2win.vip/products/tomhorn/web/incas-treasure.png</t>
+  </si>
+  <si>
+    <t>413  Game Provider Name = RelaxGaming   Game Name =  Iron Bank  cod = 404   src = https://resources.bet2win.vip/products/outcomebet/ironbank_rg.jpg</t>
+  </si>
+  <si>
+    <t>436  Game Provider Name = TomHorn   Game Name =  Joker Reelz  cod = 404   src = https://resources.bet2win.vip/products/tomhorn/web/joker-reelz.png</t>
+  </si>
+  <si>
+    <t>473  Game Provider Name = QuickSpin   Game Name =  Leprechaun Hills  cod = 404   src = https://resources.bet2win.vip/products/outcomebet/web/qso_leprechaunhills.jpg</t>
+  </si>
+  <si>
+    <t>514  Game Provider Name = QuickSpin   Game Name =  Mayana  cod = 404   src = https://resources.bet2win.vip/products/outcomebet/web/qso_mayana.jpg</t>
+  </si>
+  <si>
+    <t>527  Game Provider Name = QuickSpin   Game Name =  Mighty Arthur  cod = 404   src = https://resources.bet2win.vip/products/outcomebet/web/qso_mightyarthur.jpg</t>
+  </si>
+  <si>
+    <t>533  Game Provider Name = RelaxGaming   Game Name =  Money Train 2  cod = 404   src = https://resources.bet2win.vip/products/outcomebet/moneytrain2_rg.jpg</t>
+  </si>
+  <si>
+    <t>534  Game Provider Name = TomHorn   Game Name =  Monkey 27  cod = 404   src = https://resources.bet2win.vip/products/tomhorn/web/Monkey27.png</t>
+  </si>
+  <si>
+    <t>538  Game Provider Name = TomHorn   Game Name =  Monster Madness  cod = 404   src = https://resources.bet2win.vip/products/tomhorn/web/MonsterMadness.png</t>
+  </si>
+  <si>
+    <t>544  Game Provider Name = QuickSpin   Game Name =  Mountain King  cod = 404   src = https://resources.bet2win.vip/products/outcomebet/web/MountainKing.png</t>
+  </si>
+  <si>
+    <t>560  Game Provider Name = QuickSpin   Game Name =  Northern Sky  cod = 404   src = https://resources.bet2win.vip/products/outcomebet/web/NorthernSky.png</t>
+  </si>
+  <si>
+    <t>571  Game Provider Name = TomHorn   Game Name =  Panda's Run  cod = 404   src = https://resources.bet2win.vip/products/tomhorn/web/PandasRun.png</t>
+  </si>
+  <si>
+    <t>584  Game Provider Name = QuickSpin   Game Name =  Phoenix Sun  cod = 404   src = https://resources.bet2win.vip/products/outcomebet/web/qso_phoenixsun.jpg</t>
+  </si>
+  <si>
+    <t>585  Game Provider Name = QuickSpin   Game Name =  Pied Piper  cod = 404   src = https://resources.bet2win.vip/products/outcomebet/web/PiedPiper.png</t>
+  </si>
+  <si>
+    <t>593  Game Provider Name = QuickSpin   Game Name =  Pirates Charm  cod = 404   src = https://resources.bet2win.vip/products/outcomebet/web/PiratesCharm.png</t>
+  </si>
+  <si>
+    <t>625  Game Provider Name = QuickSpin   Game Name =  Razortooth  cod = 404   src = https://resources.bet2win.vip/products/outcomebet/web/qso_sabretooth.jpg</t>
+  </si>
+  <si>
+    <t>628  Game Provider Name = TomHorn   Game Name =  Red Lights  cod = 404   src = https://resources.bet2win.vip/products/tomhorn/web/RedLights.png</t>
+  </si>
+  <si>
+    <t>679  Game Provider Name = TomHorn   Game Name =  Savannah King  cod = 404   src = https://resources.bet2win.vip/products/tomhorn/web/SavannahKing.png</t>
+  </si>
+  <si>
+    <t>680  Game Provider Name = TomHorn   Game Name =  Scratch Card  cod = 404   src = https://resources.bet2win.vip/products/tomhorn/web/ScratchCard.png</t>
+  </si>
+  <si>
+    <t>685  Game Provider Name = QuickSpin   Game Name =  Second Strike  cod = 404   src = https://resources.bet2win.vip/products/outcomebet/web/qso_secondstrike.jpg</t>
+  </si>
+  <si>
+    <t>692  Game Provider Name = QuickSpin   Game Name =  Sevens High  cod = 404   src = https://resources.bet2win.vip/products/outcomebet/web/qso_sevens.jpg</t>
+  </si>
+  <si>
+    <t>695  Game Provider Name = TomHorn   Game Name =  Shaolin's Tiger  cod = 404   src = https://resources.bet2win.vip/products/tomhorn/web/ShaolinsTiger.jpg</t>
+  </si>
+  <si>
+    <t>697  Game Provider Name = TomHorn   Game Name =  Sherlock in Bohemia  cod = 404   src = https://resources.bet2win.vip/products/tomhorn/web/Sherlock.png</t>
+  </si>
+  <si>
+    <t>701  Game Provider Name = TomHorn   Game Name =  Sizable Win  cod = 404   src = https://resources.bet2win.vip/products/tomhorn/web/SizableWin.png</t>
+  </si>
+  <si>
+    <t>705  Game Provider Name = TomHorn   Game Name =  Sky Barons  cod = 404   src = https://resources.bet2win.vip/products/tomhorn/web/SkyBarons.png</t>
+  </si>
+  <si>
+    <t>708  Game Provider Name = RelaxGaming   Game Name =  Snake Arena  cod = 404   src = https://resources.bet2win.vip/products/outcomebet/snakearena_rg.jpg</t>
+  </si>
+  <si>
+    <t>721  Game Provider Name = TomHorn   Game Name =  Spinball  cod = 404   src = https://resources.bet2win.vip/products/tomhorn/web/spinball.png</t>
+  </si>
+  <si>
+    <t>722  Game Provider Name = QuickSpin   Game Name =  Spinions Beach Party  cod = 404   src = https://resources.bet2win.vip/products/outcomebet/web/qso_spinions.jpg</t>
+  </si>
+  <si>
+    <t>732  Game Provider Name = QuickSpin   Game Name =  Sticky Bandits  cod = 404   src = https://resources.bet2win.vip/products/outcomebet/web/qso_stickybandits.jpg</t>
+  </si>
+  <si>
+    <t>749  Game Provider Name = TomHorn   Game Name =  Sweet Crush  cod = 404   src = https://resources.bet2win.vip/products/tomhorn/web/sweet-crush.png</t>
+  </si>
+  <si>
+    <t>757  Game Provider Name = QuickSpin   Game Name =  Tales of Doctor Dolittle  cod = 404   src = https://resources.bet2win.vip/products/outcomebet/web/TalesofDoctorDolittle.png</t>
+  </si>
+  <si>
+    <t>762  Game Provider Name = TomHorn   Game Name =  The Cup  cod = 404   src = https://resources.bet2win.vip/products/tomhorn/web/TheCup.png</t>
+  </si>
+  <si>
+    <t>786  Game Provider Name = TomHorn   Game Name =  The Secret of BA  cod = 404   src = https://resources.bet2win.vip/products/tomhorn/web/the-secret-of-ba.png</t>
+  </si>
+  <si>
+    <t>794  Game Provider Name = TomHorn   Game Name =  Thrones Of Persia  cod = 404   src = https://resources.bet2win.vip/products/tomhorn/web/ThronesOfPersia.png</t>
+  </si>
+  <si>
+    <t>839  Game Provider Name = QuickSpin   Game Name =  Volcano Riches  cod = 404   src = https://resources.bet2win.vip/products/outcomebet/web/VolcanoRiches.png</t>
+  </si>
+  <si>
+    <t>850  Game Provider Name = RelaxGaming   Game Name =  Wild Chapo  cod = 404   src = https://resources.bet2win.vip/products/outcomebet/wildchapo_rg.jpg</t>
+  </si>
+  <si>
+    <t>852  Game Provider Name = QuickSpin   Game Name =  Wild Chase  cod = 404   src = https://resources.bet2win.vip/products/outcomebet/web/WildChase.png</t>
+  </si>
+  <si>
+    <t>866  Game Provider Name = TomHorn   Game Name =  Wild Weather  cod = 404   src = https://resources.bet2win.vip/products/tomhorn/web/WildWeather.png</t>
+  </si>
+  <si>
+    <t>874  Game Provider Name = QuickSpin   Game Name =  Wins of Fortune  cod = 404   src = https://resources.bet2win.vip/products/outcomebet/web/WinsofFortune.png</t>
+  </si>
+  <si>
+    <t>878  Game Provider Name = TomHorn   Game Name =  Wolf Sierra  cod = 404   src = https://resources.bet2win.vip/products/tomhorn/web/wolf-sierra.png</t>
   </si>
 </sst>
 </file>

</xml_diff>